<commit_message>
Update of Testcases Class MultiBrowser new Version2
</commit_message>
<xml_diff>
--- a/AddUserTCs.xlsx
+++ b/AddUserTCs.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZTE_testing\IdeaProjects\WebDriverTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A999AD1C-5B52-409F-A2B5-A8D8647D4C71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA07016-692D-4F56-82AD-301F523C1352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4830" activeTab="3" xr2:uid="{3515CBF1-68F9-44DD-B169-2F40063D1F63}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4830" firstSheet="1" activeTab="6" xr2:uid="{3515CBF1-68F9-44DD-B169-2F40063D1F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="11" r:id="rId1"/>
     <sheet name="HTTP_LINK" sheetId="7" r:id="rId2"/>
     <sheet name="Admin" sheetId="2" r:id="rId3"/>
     <sheet name="UserLogin" sheetId="10" r:id="rId4"/>
-    <sheet name="User" sheetId="1" r:id="rId5"/>
+    <sheet name="User" sheetId="12" r:id="rId5"/>
     <sheet name="modifyUser" sheetId="9" r:id="rId6"/>
     <sheet name="deleteUser" sheetId="3" r:id="rId7"/>
     <sheet name="deleteAdmin" sheetId="8" r:id="rId8"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
   <si>
     <t>TC</t>
   </si>
@@ -129,24 +129,6 @@
     <t>DeleteUser</t>
   </si>
   <si>
-    <t>nase10</t>
-  </si>
-  <si>
-    <t>nase11</t>
-  </si>
-  <si>
-    <t>nase12</t>
-  </si>
-  <si>
-    <t>nase13</t>
-  </si>
-  <si>
-    <t>DeletUser</t>
-  </si>
-  <si>
-    <t>istnichtda</t>
-  </si>
-  <si>
     <t>zz_nase1</t>
   </si>
   <si>
@@ -189,15 +171,9 @@
     <t>Value</t>
   </si>
   <si>
-    <t>loginUser_LoginName</t>
-  </si>
-  <si>
     <t>zz_nase8@emailgehtnicht.de</t>
   </si>
   <si>
-    <t>loginUser_LoginEmail</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
@@ -208,6 +184,42 @@
   </si>
   <si>
     <t>Firefox</t>
+  </si>
+  <si>
+    <t>addUserRole</t>
+  </si>
+  <si>
+    <t>zz_nase</t>
+  </si>
+  <si>
+    <t>loginUser_LoginName_Passwd(Stark)</t>
+  </si>
+  <si>
+    <t>loginUser_LoginEmail_Passwd(Mittel)</t>
+  </si>
+  <si>
+    <t>loginUser_LoginName_Passwd(Schwach)</t>
+  </si>
+  <si>
+    <t>$_1234%!zz_nase7</t>
+  </si>
+  <si>
+    <t>zz_doesnotexist</t>
+  </si>
+  <si>
+    <t>DoesnotExist</t>
+  </si>
+  <si>
+    <t>loginUser_LoginName(Exist)_Passwd(Wrong)</t>
+  </si>
+  <si>
+    <t>$_1234</t>
+  </si>
+  <si>
+    <t>loginUser_LoginName(Wrong)</t>
+  </si>
+  <si>
+    <t>DeleteUser(Several)</t>
   </si>
 </sst>
 </file>
@@ -230,12 +242,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,14 +268,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,22 +603,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -678,17 +699,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B095D3-5EBE-42FA-A099-ADD4BC840131}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -709,54 +730,88 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -765,20 +820,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2319A7-BCE9-48A9-A6B8-EB40BFCC1D02}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF4B3B2-85AF-46F6-B39B-6E458355D909}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,12 +865,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>"userAdd_"&amp; H2 &amp; "PassWD_Stark"</f>
-        <v>userAdd_MitarbeiterPassWD_Stark</v>
+      <c r="A2" t="s">
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="str">
         <f>B2&amp;"@emailgehtnicht.de"</f>
@@ -837,12 +893,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A8" si="0">"userAdd_"&amp; H3 &amp; "PassWD_Stark"</f>
-        <v>userAdd_AbonnentPassWD_Stark</v>
+      <c r="A3" t="s">
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C3" t="str">
         <f>B3&amp;"@emailgehtnicht.de"</f>
@@ -855,7 +910,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F8" si="1">"$_1234%!"&amp;B3</f>
+        <f t="shared" ref="F3:F8" si="0">"$_1234%!"&amp;B3</f>
         <v>$_1234%!zz_nase2</v>
       </c>
       <c r="G3" s="2" t="b">
@@ -866,12 +921,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>userAdd_AutorPassWD_Stark</v>
+      <c r="A4" t="s">
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" t="str">
         <f>B4&amp;"@emailgehtnicht.de"</f>
@@ -884,7 +938,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>$_1234%!zz_nase3</v>
       </c>
       <c r="G4" s="2" t="b">
@@ -895,12 +949,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>userAdd_RedakteurPassWD_Stark</v>
+      <c r="A5" t="s">
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C5" t="str">
         <f>B5&amp;"@emailgehtnicht.de"</f>
@@ -913,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>$_1234%!zz_nase4</v>
       </c>
       <c r="G5" s="2" t="b">
@@ -924,12 +977,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>userAdd_MitarbeiterPassWD_Stark</v>
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C6" t="str">
         <f>B6&amp;"@emailgehtnicht.de"</f>
@@ -942,7 +994,7 @@
         <v>19</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>$_1234%!zz_nase5</v>
       </c>
       <c r="G6" s="2" t="b">
@@ -953,15 +1005,14 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f t="shared" si="0"/>
-        <v>userAdd_AbonnentPassWD_Stark</v>
+      <c r="A7" t="s">
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" ref="C7:C10" si="2">B7&amp;"@emailgehtnicht.de"</f>
+        <f t="shared" ref="C7:C10" si="1">B7&amp;"@emailgehtnicht.de"</f>
         <v>zz_nase6@emailgehtnicht.de</v>
       </c>
       <c r="D7" t="s">
@@ -971,7 +1022,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>$_1234%!zz_nase6</v>
       </c>
       <c r="G7" s="2" t="b">
@@ -982,15 +1033,14 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>userAdd_AutorPassWD_Stark</v>
+      <c r="A8" t="s">
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zz_nase7@emailgehtnicht.de</v>
       </c>
       <c r="D8" t="s">
@@ -1000,7 +1050,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>$_1234%!zz_nase7</v>
       </c>
       <c r="G8" s="2" t="b">
@@ -1011,15 +1061,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>"userAdd_"&amp; H9&amp;"PassWD_Schwach"</f>
-        <v>userAdd_RedakteurPassWD_Schwach</v>
+      <c r="A9" t="s">
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zz_nase8@emailgehtnicht.de</v>
       </c>
       <c r="D9" t="s">
@@ -1029,7 +1078,7 @@
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>0</v>
@@ -1039,15 +1088,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>"userAdd_"&amp; H10&amp;"PassWD_GanzSchwach"</f>
-        <v>userAdd_MitarbeiterPassWD_GanzSchwach</v>
+      <c r="A10" t="s">
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>zz_nase9@emailgehtnicht.de</v>
       </c>
       <c r="D10" t="s">
@@ -1057,7 +1105,7 @@
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>0</v>
@@ -1066,12 +1114,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G12" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1080,7 +1124,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,26 +1141,26 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1124,10 +1168,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1135,10 +1179,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1146,10 +1190,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
@@ -1162,15 +1206,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2176393-849F-4A80-8E94-27A38EAB00FF}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1195,39 +1239,15 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>